<commit_message>
fixed xls input issue
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="35">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -131,9 +131,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -215,8 +216,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,7 +229,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,20 +254,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.42"/>
@@ -271,61 +280,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -333,7 +342,7 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="b">
+      <c r="B2" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -355,7 +364,7 @@
       <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="b">
+      <c r="I2" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -394,7 +403,7 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -416,7 +425,7 @@
       <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="b">
+      <c r="I3" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -455,7 +464,7 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -477,7 +486,7 @@
       <c r="H4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="2" t="b">
+      <c r="I4" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -516,7 +525,7 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -538,7 +547,7 @@
       <c r="H5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2" t="b">
+      <c r="I5" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -577,7 +586,7 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -599,7 +608,7 @@
       <c r="H6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="2" t="b">
+      <c r="I6" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -638,7 +647,7 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -660,7 +669,7 @@
       <c r="H7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="2" t="b">
+      <c r="I7" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -699,7 +708,7 @@
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -721,7 +730,7 @@
       <c r="H8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="2" t="b">
+      <c r="I8" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -760,7 +769,7 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -782,7 +791,7 @@
       <c r="H9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="2" t="b">
+      <c r="I9" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -821,7 +830,7 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -843,7 +852,7 @@
       <c r="H10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="2" t="b">
+      <c r="I10" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -882,7 +891,7 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -904,7 +913,7 @@
       <c r="H11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="2" t="b">
+      <c r="I11" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -943,7 +952,7 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -965,7 +974,7 @@
       <c r="H12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="2" t="b">
+      <c r="I12" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1004,7 +1013,7 @@
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1026,7 +1035,7 @@
       <c r="H13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="2" t="b">
+      <c r="I13" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1065,7 +1074,7 @@
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="b">
+      <c r="B14" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1084,7 +1093,7 @@
       <c r="H14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="2" t="b">
+      <c r="I14" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1123,7 +1132,7 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="b">
+      <c r="B15" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1142,7 +1151,7 @@
       <c r="H15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="2" t="b">
+      <c r="I15" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1181,7 +1190,7 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="b">
+      <c r="B16" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1200,7 +1209,7 @@
       <c r="H16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="2" t="b">
+      <c r="I16" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1239,7 +1248,7 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="b">
+      <c r="B17" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1258,7 +1267,7 @@
       <c r="H17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="2" t="b">
+      <c r="I17" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1297,7 +1306,7 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="b">
+      <c r="B18" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1316,7 +1325,7 @@
       <c r="H18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="2" t="b">
+      <c r="I18" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1355,7 +1364,7 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="b">
+      <c r="B19" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1374,7 +1383,7 @@
       <c r="H19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="2" t="b">
+      <c r="I19" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1413,7 +1422,7 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="b">
+      <c r="B20" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1432,7 +1441,7 @@
       <c r="H20" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="2" t="b">
+      <c r="I20" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1471,7 +1480,7 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="b">
+      <c r="B21" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1490,7 +1499,7 @@
       <c r="H21" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="2" t="b">
+      <c r="I21" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1529,7 +1538,7 @@
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="b">
+      <c r="B22" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1548,7 +1557,7 @@
       <c r="H22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="2" t="b">
+      <c r="I22" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1587,7 +1596,7 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="b">
+      <c r="B23" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1606,7 +1615,7 @@
       <c r="H23" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="2" t="b">
+      <c r="I23" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1645,7 +1654,7 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="b">
+      <c r="B24" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1664,7 +1673,7 @@
       <c r="H24" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="2" t="b">
+      <c r="I24" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1703,7 +1712,7 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="b">
+      <c r="B25" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1722,7 +1731,7 @@
       <c r="H25" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="2" t="b">
+      <c r="I25" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1761,7 +1770,7 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="b">
+      <c r="B26" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1783,7 +1792,7 @@
       <c r="H26" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="2" t="b">
+      <c r="I26" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1822,7 +1831,7 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="b">
+      <c r="B27" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1844,7 +1853,7 @@
       <c r="H27" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="2" t="b">
+      <c r="I27" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1883,7 +1892,7 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="b">
+      <c r="B28" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1905,7 +1914,7 @@
       <c r="H28" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="2" t="b">
+      <c r="I28" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1944,7 +1953,7 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="b">
+      <c r="B29" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1966,7 +1975,7 @@
       <c r="H29" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="2" t="b">
+      <c r="I29" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="b">
+      <c r="B30" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2027,7 +2036,7 @@
       <c r="H30" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="2" t="b">
+      <c r="I30" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2066,7 +2075,7 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="b">
+      <c r="B31" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2088,7 +2097,7 @@
       <c r="H31" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="2" t="b">
+      <c r="I31" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2127,7 +2136,7 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="b">
+      <c r="B32" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2149,7 +2158,7 @@
       <c r="H32" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="2" t="b">
+      <c r="I32" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2188,7 +2197,7 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="b">
+      <c r="B33" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2210,7 +2219,7 @@
       <c r="H33" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="2" t="b">
+      <c r="I33" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2249,7 +2258,7 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="b">
+      <c r="B34" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2271,7 +2280,7 @@
       <c r="H34" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="2" t="b">
+      <c r="I34" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2304,6 +2313,354 @@
       </c>
       <c r="S34" s="0" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q35" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q36" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q37" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>0.935239</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few bug fixes.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="36">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">util_room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +240,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,10 +261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +432,7 @@
       <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="b">
+      <c r="I3" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -486,7 +493,7 @@
       <c r="H4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="4" t="b">
+      <c r="I4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -547,7 +554,7 @@
       <c r="H5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="4" t="b">
+      <c r="I5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -608,7 +615,7 @@
       <c r="H6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="4" t="b">
+      <c r="I6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -669,7 +676,7 @@
       <c r="H7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="4" t="b">
+      <c r="I7" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -730,7 +737,7 @@
       <c r="H8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="4" t="b">
+      <c r="I8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -791,7 +798,7 @@
       <c r="H9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="4" t="b">
+      <c r="I9" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -852,7 +859,7 @@
       <c r="H10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="4" t="b">
+      <c r="I10" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -913,7 +920,7 @@
       <c r="H11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="4" t="b">
+      <c r="I11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -974,7 +981,7 @@
       <c r="H12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="4" t="b">
+      <c r="I12" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1035,7 +1042,7 @@
       <c r="H13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="4" t="b">
+      <c r="I13" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1093,7 +1100,7 @@
       <c r="H14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="4" t="b">
+      <c r="I14" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1132,7 +1139,7 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="b">
+      <c r="B15" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1151,7 +1158,7 @@
       <c r="H15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="4" t="b">
+      <c r="I15" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1171,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>0.534208</v>
+        <v>0.53</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>0.98</v>
@@ -1190,7 +1197,7 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="b">
+      <c r="B16" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1209,7 +1216,7 @@
       <c r="H16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="4" t="b">
+      <c r="I16" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>0.534208</v>
+        <v>0.53</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>0.98</v>
@@ -1248,12 +1255,12 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="b">
+      <c r="B17" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -1267,7 +1274,7 @@
       <c r="H17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="4" t="b">
+      <c r="I17" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>33</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="0" t="s">
         <v>23</v>
@@ -1306,12 +1313,12 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="b">
+      <c r="B18" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -1325,7 +1332,7 @@
       <c r="H18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="4" t="b">
+      <c r="I18" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>0.03</v>
+        <v>0.29</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>0.98</v>
@@ -1354,7 +1361,7 @@
         <v>24</v>
       </c>
       <c r="R18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="0" t="s">
         <v>23</v>
@@ -1364,12 +1371,12 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="b">
+      <c r="B19" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>1</v>
@@ -1383,7 +1390,7 @@
       <c r="H19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="4" t="b">
+      <c r="I19" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>0.03</v>
+        <v>0.29</v>
       </c>
       <c r="P19" s="0" t="n">
         <v>0.98</v>
@@ -1422,12 +1429,12 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="b">
+      <c r="B20" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -1441,7 +1448,7 @@
       <c r="H20" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="4" t="b">
+      <c r="I20" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1449,7 +1456,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>20</v>
@@ -1464,28 +1471,28 @@
         <v>0.7</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>-0.12</v>
+        <v>0.98</v>
       </c>
       <c r="Q20" s="0" t="s">
         <v>33</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="b">
+      <c r="B21" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -1499,7 +1506,7 @@
       <c r="H21" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="4" t="b">
+      <c r="I21" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>29</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>20</v>
@@ -1519,10 +1526,10 @@
         <v>1</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>0.534208</v>
+        <v>0.03</v>
       </c>
       <c r="P21" s="0" t="n">
-        <v>-0.12</v>
+        <v>0.98</v>
       </c>
       <c r="Q21" s="0" t="s">
         <v>24</v>
@@ -1531,19 +1538,19 @@
         <v>0</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="b">
+      <c r="B22" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1</v>
@@ -1557,7 +1564,7 @@
       <c r="H22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="4" t="b">
+      <c r="I22" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1565,7 +1572,7 @@
         <v>29</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>20</v>
@@ -1577,31 +1584,31 @@
         <v>1</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>0.534208</v>
+        <v>0.03</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="Q22" s="0" t="s">
         <v>25</v>
       </c>
       <c r="R22" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="b">
+      <c r="B23" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>1</v>
@@ -1613,9 +1620,9 @@
         <v>28</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I23" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>29</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>20</v>
@@ -1638,28 +1645,28 @@
         <v>0.7</v>
       </c>
       <c r="P23" s="0" t="n">
-        <v>0.8</v>
+        <v>-0.12</v>
       </c>
       <c r="Q23" s="0" t="s">
         <v>33</v>
       </c>
       <c r="R23" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="b">
+      <c r="B24" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -1671,9 +1678,9 @@
         <v>28</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I24" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>29</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>20</v>
@@ -1693,10 +1700,10 @@
         <v>1</v>
       </c>
       <c r="O24" s="0" t="n">
-        <v>0.03</v>
+        <v>0.53</v>
       </c>
       <c r="P24" s="0" t="n">
-        <v>0.8</v>
+        <v>-0.12</v>
       </c>
       <c r="Q24" s="0" t="s">
         <v>24</v>
@@ -1705,19 +1712,19 @@
         <v>0</v>
       </c>
       <c r="S24" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="b">
+      <c r="B25" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
@@ -1729,9 +1736,9 @@
         <v>28</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I25" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1739,7 +1746,7 @@
         <v>29</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>20</v>
@@ -1751,34 +1758,31 @@
         <v>1</v>
       </c>
       <c r="O25" s="0" t="n">
-        <v>0.03</v>
+        <v>0.53</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="0" t="s">
         <v>25</v>
       </c>
       <c r="R25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>19</v>
+      <c r="B26" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>
@@ -1787,59 +1791,56 @@
         <v>0</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="I26" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M26" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>1</v>
+        <v>-0.7</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>0.98</v>
+        <v>0.8</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>19</v>
+      <c r="B27" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>1</v>
@@ -1848,35 +1849,35 @@
         <v>0</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="I27" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M27" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>0.98</v>
+        <v>0.8</v>
       </c>
       <c r="Q27" s="0" t="s">
         <v>24</v>
@@ -1885,22 +1886,19 @@
         <v>0</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>19</v>
+      <c r="B28" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
@@ -1909,56 +1907,56 @@
         <v>0</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="I28" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M28" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>0.98</v>
+        <v>0.8</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="R28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="b">
+      <c r="B29" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -1970,17 +1968,17 @@
         <v>0</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I29" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="K29" s="0" t="n">
         <v>70</v>
@@ -2014,12 +2012,12 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="b">
+      <c r="B30" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -2031,12 +2029,12 @@
         <v>0</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I30" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2075,12 +2073,12 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="b">
+      <c r="B31" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -2092,12 +2090,12 @@
         <v>0</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="4" t="b">
+        <v>19</v>
+      </c>
+      <c r="I31" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2136,7 +2134,7 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="b">
+      <c r="B32" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2153,12 +2151,12 @@
         <v>0</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="4" t="b">
+        <v>28</v>
+      </c>
+      <c r="I32" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2197,7 +2195,7 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="b">
+      <c r="B33" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2214,12 +2212,12 @@
         <v>0</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="4" t="b">
+        <v>28</v>
+      </c>
+      <c r="I33" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2258,7 +2256,7 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="b">
+      <c r="B34" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2275,12 +2273,12 @@
         <v>0</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="4" t="b">
+        <v>28</v>
+      </c>
+      <c r="I34" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2319,104 +2317,110 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="B35" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="I35" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>70</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M35" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N35" s="0" t="n">
-        <v>-0.7</v>
+        <v>1</v>
       </c>
       <c r="O35" s="0" t="n">
-        <v>0.935239</v>
+        <v>1</v>
       </c>
       <c r="P35" s="0" t="n">
         <v>0.98</v>
       </c>
       <c r="Q35" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="S35" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="B36" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="I36" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K36" s="0" t="n">
         <v>70</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M36" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N36" s="0" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>0.935239</v>
+        <v>1</v>
       </c>
       <c r="P36" s="0" t="n">
         <v>0.98</v>
@@ -2428,83 +2432,86 @@
         <v>0</v>
       </c>
       <c r="S36" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="B37" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="4" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="I37" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>70</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="M37" s="0" t="s">
         <v>21</v>
       </c>
       <c r="N37" s="0" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O37" s="0" t="n">
-        <v>0.935239</v>
+        <v>1</v>
       </c>
       <c r="P37" s="0" t="n">
         <v>0.98</v>
       </c>
       <c r="Q37" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S37" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="b">
+      <c r="B38" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>28</v>
@@ -2512,7 +2519,7 @@
       <c r="H38" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="4" t="b">
+      <c r="I38" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>-0.7</v>
       </c>
       <c r="O38" s="0" t="n">
-        <v>0.935239</v>
+        <v>0.93</v>
       </c>
       <c r="P38" s="0" t="n">
         <v>0.98</v>
@@ -2551,18 +2558,18 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="b">
+      <c r="B39" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>28</v>
@@ -2570,7 +2577,7 @@
       <c r="H39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="4" t="b">
+      <c r="I39" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="O39" s="0" t="n">
-        <v>0.935239</v>
+        <v>0.93</v>
       </c>
       <c r="P39" s="0" t="n">
         <v>0.98</v>
@@ -2609,18 +2616,18 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="b">
+      <c r="B40" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>28</v>
@@ -2628,7 +2635,7 @@
       <c r="H40" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="4" t="b">
+      <c r="I40" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2648,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="O40" s="0" t="n">
-        <v>0.935239</v>
+        <v>0.93</v>
       </c>
       <c r="P40" s="0" t="n">
         <v>0.98</v>
@@ -2660,6 +2667,180 @@
         <v>0</v>
       </c>
       <c r="S40" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="P42" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="5" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="P43" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" s="0" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a few tweaks and renaming.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="35">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">autonomy</t>
   </si>
   <si>
-    <t xml:space="preserve">[‘move_away’]</t>
+    <t xml:space="preserve">['move_away']</t>
   </si>
   <si>
     <t xml:space="preserve">move_away</t>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">util_room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
   </si>
 </sst>
 </file>
@@ -219,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,10 +237,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,7 +372,7 @@
         <v>20</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>20</v>
@@ -432,7 +425,7 @@
       <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="5" t="b">
+      <c r="I3" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -440,7 +433,7 @@
         <v>20</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>20</v>
@@ -493,7 +486,7 @@
       <c r="H4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="5" t="b">
+      <c r="I4" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -501,7 +494,7 @@
         <v>20</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>20</v>
@@ -554,7 +547,7 @@
       <c r="H5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="5" t="b">
+      <c r="I5" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -562,7 +555,7 @@
         <v>20</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>20</v>
@@ -615,7 +608,7 @@
       <c r="H6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="5" t="b">
+      <c r="I6" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -623,7 +616,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>20</v>
@@ -676,7 +669,7 @@
       <c r="H7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="5" t="b">
+      <c r="I7" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -684,7 +677,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>20</v>
@@ -737,7 +730,7 @@
       <c r="H8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="5" t="b">
+      <c r="I8" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -745,7 +738,7 @@
         <v>29</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>20</v>
@@ -798,7 +791,7 @@
       <c r="H9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="5" t="b">
+      <c r="I9" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -806,7 +799,7 @@
         <v>29</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>20</v>
@@ -859,7 +852,7 @@
       <c r="H10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="5" t="b">
+      <c r="I10" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -867,7 +860,7 @@
         <v>29</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>20</v>
@@ -920,7 +913,7 @@
       <c r="H11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="5" t="b">
+      <c r="I11" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -928,7 +921,7 @@
         <v>20</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>31</v>
@@ -981,7 +974,7 @@
       <c r="H12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="5" t="b">
+      <c r="I12" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -989,7 +982,7 @@
         <v>20</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>31</v>
@@ -1042,7 +1035,7 @@
       <c r="H13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="5" t="b">
+      <c r="I13" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1050,7 +1043,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>31</v>
@@ -1100,7 +1093,7 @@
       <c r="H14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="5" t="b">
+      <c r="I14" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1108,7 +1101,7 @@
         <v>29</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>20</v>
@@ -1139,7 +1132,7 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="b">
+      <c r="B15" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1158,7 +1151,7 @@
       <c r="H15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="5" t="b">
+      <c r="I15" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1166,7 +1159,7 @@
         <v>29</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>20</v>
@@ -1197,7 +1190,7 @@
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="b">
+      <c r="B16" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1216,7 +1209,7 @@
       <c r="H16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="5" t="b">
+      <c r="I16" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1224,7 +1217,7 @@
         <v>29</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>20</v>
@@ -1255,7 +1248,7 @@
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="b">
+      <c r="B17" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1274,7 +1267,7 @@
       <c r="H17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="5" t="b">
+      <c r="I17" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1282,7 +1275,7 @@
         <v>29</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>20</v>
@@ -1313,7 +1306,7 @@
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="b">
+      <c r="B18" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1332,7 +1325,7 @@
       <c r="H18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="5" t="b">
+      <c r="I18" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1340,7 +1333,7 @@
         <v>29</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>20</v>
@@ -1352,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>0.98</v>
@@ -1371,7 +1364,7 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="b">
+      <c r="B19" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1390,7 +1383,7 @@
       <c r="H19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="5" t="b">
+      <c r="I19" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1398,7 +1391,7 @@
         <v>29</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>20</v>
@@ -1410,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="P19" s="0" t="n">
         <v>0.98</v>
@@ -1429,7 +1422,7 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="b">
+      <c r="B20" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1448,7 +1441,7 @@
       <c r="H20" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="5" t="b">
+      <c r="I20" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1456,7 +1449,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>20</v>
@@ -1487,7 +1480,7 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="b">
+      <c r="B21" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1506,7 +1499,7 @@
       <c r="H21" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="5" t="b">
+      <c r="I21" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1514,7 +1507,7 @@
         <v>29</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>20</v>
@@ -1526,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="O21" s="0" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="P21" s="0" t="n">
         <v>0.98</v>
@@ -1545,7 +1538,7 @@
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="b">
+      <c r="B22" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1564,7 +1557,7 @@
       <c r="H22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="5" t="b">
+      <c r="I22" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1572,7 +1565,7 @@
         <v>29</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>20</v>
@@ -1584,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="P22" s="0" t="n">
         <v>0.98</v>
@@ -1603,7 +1596,7 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="b">
+      <c r="B23" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1622,7 +1615,7 @@
       <c r="H23" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="5" t="b">
+      <c r="I23" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1661,7 +1654,7 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="b">
+      <c r="B24" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1680,7 +1673,7 @@
       <c r="H24" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="5" t="b">
+      <c r="I24" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1719,7 +1712,7 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="b">
+      <c r="B25" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1738,7 +1731,7 @@
       <c r="H25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="5" t="b">
+      <c r="I25" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1777,7 +1770,7 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="b">
+      <c r="B26" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1796,7 +1789,7 @@
       <c r="H26" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="5" t="b">
+      <c r="I26" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1835,7 +1828,7 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="b">
+      <c r="B27" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1854,7 +1847,7 @@
       <c r="H27" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I27" s="5" t="b">
+      <c r="I27" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1874,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="O27" s="0" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="P27" s="0" t="n">
         <v>0.8</v>
@@ -1893,7 +1886,7 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="b">
+      <c r="B28" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1912,7 +1905,7 @@
       <c r="H28" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="5" t="b">
+      <c r="I28" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1932,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>0.03</v>
+        <v>-0.03</v>
       </c>
       <c r="P28" s="0" t="n">
         <v>0.8</v>
@@ -1951,7 +1944,7 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="b">
+      <c r="B29" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1973,15 +1966,15 @@
       <c r="H29" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="5" t="b">
+      <c r="I29" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L29" s="0" t="s">
         <v>31</v>
@@ -2012,7 +2005,7 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="b">
+      <c r="B30" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2034,7 +2027,7 @@
       <c r="H30" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="5" t="b">
+      <c r="I30" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2042,7 +2035,7 @@
         <v>20</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L30" s="0" t="s">
         <v>31</v>
@@ -2073,7 +2066,7 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="b">
+      <c r="B31" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2095,7 +2088,7 @@
       <c r="H31" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="5" t="b">
+      <c r="I31" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2103,7 +2096,7 @@
         <v>20</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L31" s="0" t="s">
         <v>31</v>
@@ -2134,7 +2127,7 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="b">
+      <c r="B32" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2156,7 +2149,7 @@
       <c r="H32" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="5" t="b">
+      <c r="I32" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2164,7 +2157,7 @@
         <v>20</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L32" s="0" t="s">
         <v>31</v>
@@ -2195,7 +2188,7 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="b">
+      <c r="B33" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2217,7 +2210,7 @@
       <c r="H33" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="5" t="b">
+      <c r="I33" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2225,7 +2218,7 @@
         <v>20</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L33" s="0" t="s">
         <v>31</v>
@@ -2256,7 +2249,7 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="b">
+      <c r="B34" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2278,7 +2271,7 @@
       <c r="H34" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I34" s="5" t="b">
+      <c r="I34" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2286,7 +2279,7 @@
         <v>20</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L34" s="0" t="s">
         <v>31</v>
@@ -2317,7 +2310,7 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="b">
+      <c r="B35" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2339,7 +2332,7 @@
       <c r="H35" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="5" t="b">
+      <c r="I35" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2347,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="K35" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L35" s="0" t="s">
         <v>31</v>
@@ -2378,7 +2371,7 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="b">
+      <c r="B36" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2400,7 +2393,7 @@
       <c r="H36" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="5" t="b">
+      <c r="I36" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2408,7 +2401,7 @@
         <v>20</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L36" s="0" t="s">
         <v>31</v>
@@ -2439,7 +2432,7 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="b">
+      <c r="B37" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2461,7 +2454,7 @@
       <c r="H37" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="5" t="b">
+      <c r="I37" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2469,7 +2462,7 @@
         <v>20</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L37" s="0" t="s">
         <v>31</v>
@@ -2500,12 +2493,12 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="b">
+      <c r="B38" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
@@ -2519,7 +2512,7 @@
       <c r="H38" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="5" t="b">
+      <c r="I38" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2527,7 +2520,7 @@
         <v>29</v>
       </c>
       <c r="K38" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L38" s="0" t="s">
         <v>20</v>
@@ -2548,7 +2541,7 @@
         <v>33</v>
       </c>
       <c r="R38" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" s="0" t="s">
         <v>23</v>
@@ -2558,7 +2551,7 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="b">
+      <c r="B39" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2577,7 +2570,7 @@
       <c r="H39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="5" t="b">
+      <c r="I39" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2585,7 +2578,7 @@
         <v>29</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L39" s="0" t="s">
         <v>20</v>
@@ -2594,7 +2587,7 @@
         <v>21</v>
       </c>
       <c r="N39" s="0" t="n">
-        <v>1</v>
+        <v>-0.7</v>
       </c>
       <c r="O39" s="0" t="n">
         <v>0.93</v>
@@ -2603,10 +2596,10 @@
         <v>0.98</v>
       </c>
       <c r="Q39" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="R39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S39" s="0" t="s">
         <v>23</v>
@@ -2616,7 +2609,7 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="b">
+      <c r="B40" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2635,7 +2628,7 @@
       <c r="H40" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="5" t="b">
+      <c r="I40" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2643,7 +2636,7 @@
         <v>29</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L40" s="0" t="s">
         <v>20</v>
@@ -2661,7 +2654,7 @@
         <v>0.98</v>
       </c>
       <c r="Q40" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R40" s="0" t="n">
         <v>0</v>
@@ -2674,18 +2667,18 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="b">
+      <c r="B41" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>28</v>
@@ -2693,7 +2686,7 @@
       <c r="H41" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="5" t="b">
+      <c r="I41" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2701,7 +2694,7 @@
         <v>29</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L41" s="0" t="s">
         <v>20</v>
@@ -2710,7 +2703,7 @@
         <v>21</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>-0.7</v>
+        <v>1</v>
       </c>
       <c r="O41" s="0" t="n">
         <v>0.93</v>
@@ -2719,10 +2712,10 @@
         <v>0.98</v>
       </c>
       <c r="Q41" s="0" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="R41" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" s="0" t="s">
         <v>23</v>
@@ -2732,7 +2725,7 @@
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="b">
+      <c r="B42" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2751,7 +2744,7 @@
       <c r="H42" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="5" t="b">
+      <c r="I42" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2759,7 +2752,7 @@
         <v>29</v>
       </c>
       <c r="K42" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L42" s="0" t="s">
         <v>20</v>
@@ -2768,7 +2761,7 @@
         <v>21</v>
       </c>
       <c r="N42" s="0" t="n">
-        <v>1</v>
+        <v>-0.7</v>
       </c>
       <c r="O42" s="0" t="n">
         <v>0.93</v>
@@ -2777,10 +2770,10 @@
         <v>0.98</v>
       </c>
       <c r="Q42" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="R42" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" s="0" t="s">
         <v>23</v>
@@ -2790,7 +2783,7 @@
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="b">
+      <c r="B43" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2809,7 +2802,7 @@
       <c r="H43" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="5" t="b">
+      <c r="I43" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2817,7 +2810,7 @@
         <v>29</v>
       </c>
       <c r="K43" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="L43" s="0" t="s">
         <v>20</v>
@@ -2835,12 +2828,70 @@
         <v>0.98</v>
       </c>
       <c r="Q43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="0" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="P44" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q44" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="R43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S43" s="0" t="s">
+      <c r="R44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="0" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more bedroom cases.
</commit_message>
<xml_diff>
--- a/ethical_governor/blackboard/commonutils/cbr/data.xlsx
+++ b/ethical_governor/blackboard/commonutils/cbr/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="39">
   <si>
     <t xml:space="preserve">case_id</t>
   </si>
@@ -125,6 +125,76 @@
   </si>
   <si>
     <t xml:space="preserve">util_room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bedroom_close_bed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bedroom_close_bed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">']</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">night</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bedroom_close_bed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">']</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -136,7 +206,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,6 +234,20 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -216,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +321,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,6 +338,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF6AAB73"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -254,10 +406,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -608,7 +760,7 @@
       <c r="H6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="4" t="b">
+      <c r="I6" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -669,7 +821,7 @@
       <c r="H7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="4" t="b">
+      <c r="I7" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -730,7 +882,7 @@
       <c r="H8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="4" t="b">
+      <c r="I8" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -791,7 +943,7 @@
       <c r="H9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="4" t="b">
+      <c r="I9" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -852,7 +1004,7 @@
       <c r="H10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="4" t="b">
+      <c r="I10" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -913,7 +1065,7 @@
       <c r="H11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="4" t="b">
+      <c r="I11" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -974,7 +1126,7 @@
       <c r="H12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="4" t="b">
+      <c r="I12" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1035,7 +1187,7 @@
       <c r="H13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="4" t="b">
+      <c r="I13" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1093,7 +1245,7 @@
       <c r="H14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="4" t="b">
+      <c r="I14" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1151,7 +1303,7 @@
       <c r="H15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="4" t="b">
+      <c r="I15" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1209,7 +1361,7 @@
       <c r="H16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="4" t="b">
+      <c r="I16" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1267,7 +1419,7 @@
       <c r="H17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="4" t="b">
+      <c r="I17" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1299,14 +1451,14 @@
         <v>0</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="b">
+      <c r="B18" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1325,7 +1477,7 @@
       <c r="H18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="4" t="b">
+      <c r="I18" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1357,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,7 +1748,7 @@
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="b">
+      <c r="B23" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1615,7 +1767,7 @@
       <c r="H23" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="4" t="b">
+      <c r="I23" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1654,7 +1806,7 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="b">
+      <c r="B24" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1673,7 +1825,7 @@
       <c r="H24" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="4" t="b">
+      <c r="I24" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1712,7 +1864,7 @@
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="b">
+      <c r="B25" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1731,7 +1883,7 @@
       <c r="H25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="4" t="b">
+      <c r="I25" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1770,7 +1922,7 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="b">
+      <c r="B26" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1789,7 +1941,7 @@
       <c r="H26" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I26" s="4" t="b">
+      <c r="I26" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1828,7 +1980,7 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="b">
+      <c r="B27" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1847,7 +1999,7 @@
       <c r="H27" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I27" s="4" t="b">
+      <c r="I27" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1886,7 +2038,7 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="b">
+      <c r="B28" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1905,7 +2057,7 @@
       <c r="H28" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="4" t="b">
+      <c r="I28" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1944,7 +2096,7 @@
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="b">
+      <c r="B29" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1963,7 +2115,7 @@
       <c r="H29" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="4" t="b">
+      <c r="I29" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2002,7 +2154,7 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="b">
+      <c r="B30" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2021,7 +2173,7 @@
       <c r="H30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="4" t="b">
+      <c r="I30" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2060,7 +2212,7 @@
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="b">
+      <c r="B31" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2079,7 +2231,7 @@
       <c r="H31" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I31" s="4" t="b">
+      <c r="I31" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2118,7 +2270,7 @@
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="b">
+      <c r="B32" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2140,7 +2292,7 @@
       <c r="H32" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="4" t="b">
+      <c r="I32" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2179,7 +2331,7 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="b">
+      <c r="B33" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2201,7 +2353,7 @@
       <c r="H33" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="4" t="b">
+      <c r="I33" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2240,7 +2392,7 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="b">
+      <c r="B34" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2262,7 +2414,7 @@
       <c r="H34" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="4" t="b">
+      <c r="I34" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2301,7 +2453,7 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="b">
+      <c r="B35" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2323,7 +2475,7 @@
       <c r="H35" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="4" t="b">
+      <c r="I35" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2362,7 +2514,7 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="b">
+      <c r="B36" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2384,7 +2536,7 @@
       <c r="H36" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="4" t="b">
+      <c r="I36" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2423,7 +2575,7 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="b">
+      <c r="B37" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2445,7 +2597,7 @@
       <c r="H37" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="4" t="b">
+      <c r="I37" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2484,7 +2636,7 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="b">
+      <c r="B38" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2506,7 +2658,7 @@
       <c r="H38" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="4" t="b">
+      <c r="I38" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2545,7 +2697,7 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="b">
+      <c r="B39" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2567,7 +2719,7 @@
       <c r="H39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="4" t="b">
+      <c r="I39" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2606,7 +2758,7 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="b">
+      <c r="B40" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2628,7 +2780,7 @@
       <c r="H40" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="4" t="b">
+      <c r="I40" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2667,7 +2819,7 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="b">
+      <c r="B41" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2686,7 +2838,7 @@
       <c r="H41" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="4" t="b">
+      <c r="I41" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2725,7 +2877,7 @@
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="b">
+      <c r="B42" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2744,7 +2896,7 @@
       <c r="H42" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="4" t="b">
+      <c r="I42" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2783,7 +2935,7 @@
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="b">
+      <c r="B43" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2802,7 +2954,7 @@
       <c r="H43" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="4" t="b">
+      <c r="I43" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2841,7 +2993,7 @@
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="b">
+      <c r="B44" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2860,7 +3012,7 @@
       <c r="H44" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="4" t="b">
+      <c r="I44" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2899,7 +3051,7 @@
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="b">
+      <c r="B45" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2918,7 +3070,7 @@
       <c r="H45" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="4" t="b">
+      <c r="I45" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2957,7 +3109,7 @@
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="b">
+      <c r="B46" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2976,7 +3128,7 @@
       <c r="H46" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I46" s="4" t="b">
+      <c r="I46" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3015,7 +3167,7 @@
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="4" t="b">
+      <c r="B47" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3034,7 +3186,7 @@
       <c r="H47" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I47" s="4" t="b">
+      <c r="I47" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3067,6 +3219,180 @@
       </c>
       <c r="S47" s="0" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="0" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" s="0" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P48" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q48" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="R48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="0" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P49" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S49" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="0" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="Q50" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>